<commit_message>
updated DriverFactory with browser fallback logic and cleanup
</commit_message>
<xml_diff>
--- a/test-data/CreateUserData.xlsx
+++ b/test-data/CreateUserData.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krishna Enterprises\eclipse-workspace\selenium-automation-framework\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ECAA8A-D72B-4A9B-B47A-22D1702F7F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1286E9F-872C-412B-BD29-AE202E610E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="UserData" sheetId="1" r:id="rId1"/>
+    <sheet name="UserData" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -380,18 +380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098331EC-492B-406C-8BCB-17BA48E1C917}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="19.33203125"/>
-    <col min="3" max="3" customWidth="true" width="17.44140625"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s" s="0">
@@ -444,6 +440,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>